<commit_message>
changed the model significantly on the part of the efficiencies.
I have added graphical functions instead of the stock and flow structure. The stock and flows are actually now not deleted but they don't make much sense. so I will talk to Anna about this and potentially change it . it makes so much more sense liek this :+1:
</commit_message>
<xml_diff>
--- a/input data.xlsx
+++ b/input data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h85600_IVe003\Documents\GitHub\HubsModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F684A5F3-C27E-49F9-857D-B72489C2BAF9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE352DC-8CAB-4FD9-B830-0A262D14F3B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EB1ED7CE-675A-4059-918E-E5ADB00B592A}"/>
   </bookViews>
@@ -63097,7 +63097,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
input data and interface update
</commit_message>
<xml_diff>
--- a/input data.xlsx
+++ b/input data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h85600_IVe003\Documents\GitHub\HubsModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0CE16C-DD70-4ACF-8E9A-A975E88C880C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0EC5D7-73F0-490A-A2B7-F9A769CBDD7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EB1ED7CE-675A-4059-918E-E5ADB00B592A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>Time</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>Base scenario</t>
-  </si>
-  <si>
-    <t>Silly scenarios</t>
   </si>
   <si>
     <t>INITIAL LSP WILLING ADOPTERS</t>
@@ -260,7 +257,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,18 +294,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -322,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -346,14 +331,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -697,100 +678,100 @@
   <sheetData>
     <row r="1" spans="1:32" s="1" customFormat="1" ht="297" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -983,10 +964,10 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -994,14 +975,14 @@
       <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -1052,7 +1033,7 @@
         <v>28</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -63111,10 +63092,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC001493-4A87-403D-9C28-93D8FE5ADA85}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63123,7 +63104,7 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -63131,42 +63112,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>7</v>
-      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -63181,26 +63142,8 @@
       <c r="D4">
         <v>65000</v>
       </c>
-      <c r="E4">
-        <v>65000</v>
-      </c>
-      <c r="F4">
-        <v>65000</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>65000</v>
-      </c>
-      <c r="I4">
-        <v>65000</v>
-      </c>
-      <c r="J4">
-        <v>65000</v>
-      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -63215,26 +63158,8 @@
       <c r="D5">
         <v>6</v>
       </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-      <c r="H5">
-        <v>6</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>6</v>
-      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -63249,26 +63174,8 @@
       <c r="D6">
         <v>300000</v>
       </c>
-      <c r="E6">
-        <v>300000</v>
-      </c>
-      <c r="F6">
-        <v>300000</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>300000</v>
-      </c>
-      <c r="I6">
-        <v>300000</v>
-      </c>
-      <c r="J6">
-        <v>300000</v>
-      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -63283,26 +63190,8 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>6</v>
-      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
@@ -63317,26 +63206,8 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="9">
-        <v>0.4</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
@@ -63351,26 +63222,8 @@
       <c r="D9">
         <v>0.6</v>
       </c>
-      <c r="E9">
-        <v>0.6</v>
-      </c>
-      <c r="F9">
-        <v>0.6</v>
-      </c>
-      <c r="G9">
-        <v>0.6</v>
-      </c>
-      <c r="H9">
-        <v>0.6</v>
-      </c>
-      <c r="I9">
-        <v>0.6</v>
-      </c>
-      <c r="J9">
-        <v>0.6</v>
-      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>7</v>
       </c>
@@ -63385,28 +63238,10 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>-0.5</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
@@ -63419,28 +63254,10 @@
       <c r="D11">
         <v>30</v>
       </c>
-      <c r="E11">
-        <v>30</v>
-      </c>
-      <c r="F11">
-        <v>30</v>
-      </c>
-      <c r="G11">
-        <v>30</v>
-      </c>
-      <c r="H11">
-        <v>30</v>
-      </c>
-      <c r="I11">
-        <v>30</v>
-      </c>
-      <c r="J11">
-        <v>30</v>
-      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
@@ -63453,26 +63270,8 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>-0.5</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -63487,26 +63286,8 @@
       <c r="D13">
         <v>5</v>
       </c>
-      <c r="E13" s="9">
-        <v>25</v>
-      </c>
-      <c r="F13">
-        <v>5</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>5</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
-      <c r="J13">
-        <v>5</v>
-      </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -63521,26 +63302,8 @@
       <c r="D14">
         <v>20</v>
       </c>
-      <c r="E14">
-        <v>20</v>
-      </c>
-      <c r="F14">
-        <v>20</v>
-      </c>
-      <c r="G14">
-        <v>20</v>
-      </c>
-      <c r="H14">
-        <v>20</v>
-      </c>
-      <c r="I14">
-        <v>20</v>
-      </c>
-      <c r="J14">
-        <v>20</v>
-      </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>10</v>
       </c>
@@ -63555,26 +63318,8 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" s="9">
-        <v>-0.5</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -63589,28 +63334,10 @@
       <c r="D16">
         <v>30</v>
       </c>
-      <c r="E16">
-        <v>30</v>
-      </c>
-      <c r="F16">
-        <v>30</v>
-      </c>
-      <c r="G16">
-        <v>30</v>
-      </c>
-      <c r="H16">
-        <v>30</v>
-      </c>
-      <c r="I16">
-        <v>30</v>
-      </c>
-      <c r="J16">
-        <v>30</v>
-      </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -63623,26 +63350,8 @@
       <c r="D17">
         <v>5</v>
       </c>
-      <c r="E17" s="9">
-        <v>35</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="H17">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>5</v>
-      </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
@@ -63657,26 +63366,8 @@
       <c r="D18" s="3">
         <v>7000000</v>
       </c>
-      <c r="E18" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="F18" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="G18" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="H18" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="I18" s="3">
-        <v>7000000</v>
-      </c>
-      <c r="J18" s="3">
-        <v>7000000</v>
-      </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>14</v>
       </c>
@@ -63691,28 +63382,10 @@
       <c r="D19">
         <v>10000</v>
       </c>
-      <c r="E19">
-        <v>10000</v>
-      </c>
-      <c r="F19">
-        <v>10000</v>
-      </c>
-      <c r="G19">
-        <v>10000</v>
-      </c>
-      <c r="H19">
-        <v>10000</v>
-      </c>
-      <c r="I19">
-        <v>10000</v>
-      </c>
-      <c r="J19">
-        <v>10000</v>
-      </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -63725,28 +63398,10 @@
       <c r="D20">
         <v>10</v>
       </c>
-      <c r="E20">
-        <v>10</v>
-      </c>
-      <c r="F20">
-        <v>10</v>
-      </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
-      <c r="H20">
-        <v>10</v>
-      </c>
-      <c r="I20">
-        <v>10</v>
-      </c>
-      <c r="J20">
-        <v>10</v>
-      </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -63759,26 +63414,8 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21" s="10">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
@@ -63793,26 +63430,8 @@
       <c r="D22">
         <v>1000</v>
       </c>
-      <c r="E22">
-        <v>100</v>
-      </c>
-      <c r="F22">
-        <v>100</v>
-      </c>
-      <c r="G22">
-        <v>100</v>
-      </c>
-      <c r="H22">
-        <v>100</v>
-      </c>
-      <c r="I22">
-        <v>100</v>
-      </c>
-      <c r="J22">
-        <v>100</v>
-      </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>17</v>
       </c>
@@ -63827,26 +63446,8 @@
       <c r="D23">
         <v>300</v>
       </c>
-      <c r="E23">
-        <v>300</v>
-      </c>
-      <c r="F23">
-        <v>300</v>
-      </c>
-      <c r="G23">
-        <v>300</v>
-      </c>
-      <c r="H23">
-        <v>300</v>
-      </c>
-      <c r="I23">
-        <v>300</v>
-      </c>
-      <c r="J23">
-        <v>300</v>
-      </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
@@ -63861,26 +63462,8 @@
       <c r="D24">
         <v>3751</v>
       </c>
-      <c r="E24">
-        <v>3751</v>
-      </c>
-      <c r="F24">
-        <v>3751</v>
-      </c>
-      <c r="G24">
-        <v>3751</v>
-      </c>
-      <c r="H24">
-        <v>3751</v>
-      </c>
-      <c r="I24" s="10">
-        <v>10000000</v>
-      </c>
-      <c r="J24">
-        <v>3751</v>
-      </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>19</v>
       </c>
@@ -63895,26 +63478,8 @@
       <c r="D25">
         <v>12</v>
       </c>
-      <c r="E25">
-        <v>12</v>
-      </c>
-      <c r="F25">
-        <v>12</v>
-      </c>
-      <c r="G25">
-        <v>12</v>
-      </c>
-      <c r="H25">
-        <v>12</v>
-      </c>
-      <c r="I25">
-        <v>12</v>
-      </c>
-      <c r="J25">
-        <v>12</v>
-      </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>20</v>
       </c>
@@ -63929,26 +63494,8 @@
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>2</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>2</v>
-      </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>21</v>
       </c>
@@ -63963,26 +63510,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27">
-        <v>24</v>
-      </c>
-      <c r="F27">
-        <v>24</v>
-      </c>
-      <c r="G27">
-        <v>24</v>
-      </c>
-      <c r="H27">
-        <v>24</v>
-      </c>
-      <c r="I27" s="10">
-        <v>72</v>
-      </c>
-      <c r="J27" s="10">
-        <v>24</v>
-      </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>22</v>
       </c>
@@ -63997,26 +63526,8 @@
       <c r="D28">
         <v>0.1</v>
       </c>
-      <c r="E28">
-        <v>0.1</v>
-      </c>
-      <c r="F28">
-        <v>0.1</v>
-      </c>
-      <c r="G28">
-        <v>0.1</v>
-      </c>
-      <c r="H28">
-        <v>0.1</v>
-      </c>
-      <c r="I28">
-        <v>0.1</v>
-      </c>
-      <c r="J28">
-        <v>0.1</v>
-      </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
@@ -64031,26 +63542,8 @@
       <c r="D29">
         <v>0.1</v>
       </c>
-      <c r="E29">
-        <v>0.1</v>
-      </c>
-      <c r="F29">
-        <v>0.1</v>
-      </c>
-      <c r="G29">
-        <v>0.1</v>
-      </c>
-      <c r="H29">
-        <v>0.1</v>
-      </c>
-      <c r="I29">
-        <v>0.1</v>
-      </c>
-      <c r="J29">
-        <v>0.1</v>
-      </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>24</v>
       </c>
@@ -64065,26 +63558,8 @@
       <c r="D30">
         <v>0.9</v>
       </c>
-      <c r="E30">
-        <v>0.9</v>
-      </c>
-      <c r="F30">
-        <v>0.9</v>
-      </c>
-      <c r="G30">
-        <v>0.9</v>
-      </c>
-      <c r="H30">
-        <v>0.9</v>
-      </c>
-      <c r="I30">
-        <v>0.9</v>
-      </c>
-      <c r="J30">
-        <v>0.9</v>
-      </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>25</v>
       </c>
@@ -64099,26 +63574,8 @@
       <c r="D31">
         <v>10000</v>
       </c>
-      <c r="E31">
-        <v>10000</v>
-      </c>
-      <c r="F31">
-        <v>10000</v>
-      </c>
-      <c r="G31">
-        <v>10000</v>
-      </c>
-      <c r="H31">
-        <v>10000</v>
-      </c>
-      <c r="I31">
-        <v>10000</v>
-      </c>
-      <c r="J31">
-        <v>10000</v>
-      </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>26</v>
       </c>
@@ -64133,26 +63590,8 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>0</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>27</v>
       </c>
@@ -64167,26 +63606,8 @@
       <c r="D33">
         <v>1</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>1</v>
-      </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>28</v>
       </c>
@@ -64201,28 +63622,10 @@
       <c r="D34">
         <v>500</v>
       </c>
-      <c r="E34">
-        <v>500</v>
-      </c>
-      <c r="F34">
-        <v>500</v>
-      </c>
-      <c r="G34">
-        <v>500</v>
-      </c>
-      <c r="H34">
-        <v>500</v>
-      </c>
-      <c r="I34">
-        <v>500</v>
-      </c>
-      <c r="J34">
-        <v>500</v>
-      </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
@@ -64235,29 +63638,8 @@
       <c r="D35">
         <v>1</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="E2:I2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>